<commit_message>
Added Advice on Resume page
</commit_message>
<xml_diff>
--- a/SourceDocuments/ResearchAroundTheWorld-Data.xlsx
+++ b/SourceDocuments/ResearchAroundTheWorld-Data.xlsx
@@ -49,7 +49,32 @@
     <t xml:space="preserve">Research Associate</t>
   </si>
   <si>
-    <t xml:space="preserve">Project manager for Ireland’s first successful marine fish hatchery. Oversaw a range of research projects covering various marine species e.g. turbot, halibut.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Molecular and population genetics of farmed strains and wild populations of turbot and halibut. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Juvenile growth and social hierarchies of flatfish. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Oversaw a range of research projects covering various marine species e.g. turbot, halibut, trout, scallops.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Marine and Freshwater Institute</t>
@@ -160,7 +185,7 @@
     <t xml:space="preserve">Bantry Marine Research Station</t>
   </si>
   <si>
-    <t xml:space="preserve">Established Ireland’s first turbot hatchery of marine fish larvae including microalgal culture, broodstock management, fertilization, metamorphosis, and juvnile growth. </t>
+    <t xml:space="preserve">Established Ireland’s first turbot hatchery of marine fish larvae including microalgal culture, broodstock management, fertilization, metamorphosis, and juvenile growth. </t>
   </si>
 </sst>
 </file>
@@ -171,7 +196,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -193,6 +218,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -249,7 +280,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -266,15 +297,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -297,13 +324,13 @@
   </sheetPr>
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="4.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="61.98"/>
@@ -329,7 +356,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="47.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="71.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -412,7 +439,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="34.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="59.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
@@ -428,7 +455,7 @@
       <c r="E6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="3" t="s">
         <v>24</v>
       </c>
     </row>
@@ -455,7 +482,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="47.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C8" s="1" t="n">
@@ -472,7 +499,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="47.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
@@ -488,11 +515,11 @@
       <c r="E9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="45.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="59.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>34</v>
       </c>
@@ -508,11 +535,11 @@
       <c r="E10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="24.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>38</v>
       </c>
@@ -528,11 +555,11 @@
       <c r="E11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="24.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
@@ -548,11 +575,11 @@
       <c r="E12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="36.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>42</v>
       </c>
@@ -568,11 +595,11 @@
       <c r="E13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="47.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>45</v>
       </c>
@@ -588,7 +615,7 @@
       <c r="E14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="3" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>